<commit_message>
BaSyX 1.5 plugin, further IDTA inconsistency
</commit_message>
<xml_diff>
--- a/platform/configuration/configuration/src/test/resources/idta/2023/IDTA 2023-0-9 _Submodel_CarbonFootprint.xlsx
+++ b/platform/configuration/configuration/src/test/resources/idta/2023/IDTA 2023-0-9 _Submodel_CarbonFootprint.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\offlineFiles\git\IIP-ecosphere\platform\platform\configuration\configuration\src\test\resources\idta\2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DACE6A7-B3DB-405D-B29C-017923B800CB}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94DBCE90-EAB7-41A4-BBFF-ABC98A70B55C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="15" windowWidth="18960" windowHeight="11325" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="18" windowWidth="18960" windowHeight="11328" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -2979,27 +2979,6 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">[SMC]
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF404040"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>PCFGoodsAddr essHandover</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF404040"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
       <t xml:space="preserve">[IRDI] 0173-1#02-ABI497#001
 </t>
     </r>
@@ -3691,17 +3670,6 @@
         <family val="2"/>
       </rPr>
       <t>Table 4: SMC Address</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF404040"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>TCFGoodsTransportAddressTakeover or TCFGoodsTransportAddressHandover</t>
     </r>
   </si>
   <si>
@@ -4955,6 +4923,13 @@
     <t>[IRDI] https://admin-shell.io/idta/CarbonFootprint/ExplanatoryStatement/1/0
 definition@en: Explanation which is needed or given so that a footprint communication can be properly understood by a purchaser, potential purchaser or user of the product
 definition@de: Erforderliche oder vorhandene Erklärung, um sicherzustellen, dass eine Fußabdruckkommunikation von einem Käufer, potenziellen Käufer oder Anwender des Produktes richtig verstanden werden kann</t>
+  </si>
+  <si>
+    <t>[SMC]
+PCFGoodsAddressHandover</t>
+  </si>
+  <si>
+    <t>TCFGoodsTransportAddressHandover or PCFGoodsAddressHandover</t>
   </si>
 </sst>
 </file>
@@ -4976,15 +4951,18 @@
       <b/>
       <sz val="16"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="20"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -4995,19 +4973,23 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -5018,6 +5000,7 @@
     <font>
       <sz val="22"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="46"/>
@@ -5213,7 +5196,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5243,6 +5226,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD9D9D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -5656,7 +5645,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -5715,6 +5704,9 @@
       <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5904,6 +5896,15 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6552,63 +6553,63 @@
       <selection sqref="A1:H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="16.5" customWidth="1"/>
-    <col min="3" max="3" width="81.5" customWidth="1"/>
-    <col min="4" max="4" width="0.6640625" customWidth="1"/>
-    <col min="5" max="5" width="8.1640625" customWidth="1"/>
+    <col min="2" max="2" width="16.46875" customWidth="1"/>
+    <col min="3" max="3" width="81.46875" customWidth="1"/>
+    <col min="4" max="4" width="0.64453125" customWidth="1"/>
+    <col min="5" max="5" width="8.17578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="150.19999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:5" ht="150.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-    </row>
-    <row r="2" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="23" t="s">
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+    </row>
+    <row r="2" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-    </row>
-    <row r="3" spans="1:5" ht="51.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="24" t="s">
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+    </row>
+    <row r="3" spans="1:5" ht="51.6" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-    </row>
-    <row r="4" spans="1:5" ht="408.95" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="5" spans="1:5" ht="408.95" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="6" spans="1:5" ht="23.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:5" ht="34.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="21" t="s">
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+    </row>
+    <row r="4" spans="1:5" ht="409" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="5" spans="1:5" ht="409" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="6" spans="1:5" ht="23.1" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="7" spans="1:5" ht="34.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-    </row>
-    <row r="8" spans="1:5" ht="116.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="20" t="s">
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+    </row>
+    <row r="8" spans="1:5" ht="116.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-    </row>
-    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+    </row>
+    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -6619,7 +6620,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="2">
         <v>45258</v>
       </c>
@@ -6630,56 +6631,56 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="21" t="s">
+    <row r="11" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-    </row>
-    <row r="12" spans="1:5" ht="299.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="20" t="s">
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+    </row>
+    <row r="12" spans="1:5" ht="299.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-    </row>
-    <row r="13" spans="1:5" ht="34.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="21" t="s">
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+    </row>
+    <row r="13" spans="1:5" ht="34.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="21"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-    </row>
-    <row r="14" spans="1:5" ht="68.849999999999994" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="20" t="s">
+      <c r="B13" s="22"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+    </row>
+    <row r="14" spans="1:5" ht="68.849999999999994" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A14" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="20"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-    </row>
-    <row r="15" spans="1:5" ht="34.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="21" t="s">
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+    </row>
+    <row r="15" spans="1:5" ht="34.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="21"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-    </row>
-    <row r="16" spans="1:5" ht="68.849999999999994" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="20" t="s">
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+    </row>
+    <row r="16" spans="1:5" ht="68.849999999999994" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A16" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="20"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -6713,195 +6714,195 @@
       <selection sqref="A1:H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="37.83203125" customWidth="1"/>
-    <col min="2" max="2" width="56.1640625" customWidth="1"/>
-    <col min="3" max="3" width="18.83203125" customWidth="1"/>
-    <col min="4" max="4" width="8.1640625" customWidth="1"/>
+    <col min="1" max="1" width="37.8203125" customWidth="1"/>
+    <col min="2" max="2" width="56.17578125" customWidth="1"/>
+    <col min="3" max="3" width="18.8203125" customWidth="1"/>
+    <col min="4" max="4" width="8.17578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="85" t="s">
+    <row r="1" spans="1:4" ht="37" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="89" t="s">
+        <v>225</v>
+      </c>
+      <c r="B1" s="89"/>
+      <c r="C1" s="89"/>
+    </row>
+    <row r="2" spans="1:4" ht="65.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="21" t="s">
+        <v>226</v>
+      </c>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+    </row>
+    <row r="3" spans="1:4" ht="153.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="21" t="s">
         <v>227</v>
       </c>
-      <c r="B1" s="85"/>
-      <c r="C1" s="85"/>
-    </row>
-    <row r="2" spans="1:4" ht="65.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="20" t="s">
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+    </row>
+    <row r="4" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="19" t="s">
         <v>228</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-    </row>
-    <row r="3" spans="1:4" ht="153.19999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="20" t="s">
+      <c r="B4" s="19" t="s">
         <v>229</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-    </row>
-    <row r="4" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="19" t="s">
+    </row>
+    <row r="5" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="10" t="s">
         <v>230</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B5" s="10" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="10" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
+      <c r="B6" s="10" t="s">
         <v>232</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
+    </row>
+    <row r="7" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B7" s="10" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="10" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="10" t="s">
+      <c r="B8" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="10" t="s">
         <v>235</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B9" s="10" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="10" t="s">
+    <row r="10" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="10" t="s">
         <v>236</v>
       </c>
-      <c r="B8" s="10" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
+      <c r="B10" s="10" t="s">
         <v>237</v>
       </c>
-      <c r="B9" s="10" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="10" t="s">
+    </row>
+    <row r="11" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="10" t="s">
         <v>238</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B11" s="10" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="10" t="s">
+    <row r="12" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="10" t="s">
         <v>240</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B12" s="10" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="10" t="s">
+    <row r="13" spans="1:4" ht="220.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="90" t="s">
         <v>242</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B13" s="90"/>
+      <c r="C13" s="90"/>
+      <c r="D13" s="90"/>
+    </row>
+    <row r="14" spans="1:4" ht="109.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A14" s="21" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="220.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="86" t="s">
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+    </row>
+    <row r="15" spans="1:4" ht="31" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="88" t="s">
         <v>244</v>
       </c>
-      <c r="B13" s="86"/>
-      <c r="C13" s="86"/>
-      <c r="D13" s="86"/>
-    </row>
-    <row r="14" spans="1:4" ht="109.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="20" t="s">
+      <c r="B15" s="88"/>
+      <c r="C15" s="88"/>
+    </row>
+    <row r="16" spans="1:4" ht="50.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A16" s="21" t="s">
         <v>245</v>
       </c>
-      <c r="B14" s="20"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-    </row>
-    <row r="15" spans="1:4" ht="30.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="84" t="s">
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+    </row>
+    <row r="17" spans="1:4" ht="50.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A17" s="21" t="s">
         <v>246</v>
       </c>
-      <c r="B15" s="84"/>
-      <c r="C15" s="84"/>
-    </row>
-    <row r="16" spans="1:4" ht="50.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="20" t="s">
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+    </row>
+    <row r="18" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A18" s="21" t="s">
         <v>247</v>
       </c>
-      <c r="B16" s="20"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-    </row>
-    <row r="17" spans="1:4" ht="50.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="20" t="s">
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+    </row>
+    <row r="19" spans="1:4" ht="50.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A19" s="21" t="s">
         <v>248</v>
       </c>
-      <c r="B17" s="20"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
-    </row>
-    <row r="18" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="20" t="s">
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+    </row>
+    <row r="20" spans="1:4" ht="77.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="21" t="s">
         <v>249</v>
       </c>
-      <c r="B18" s="20"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-    </row>
-    <row r="19" spans="1:4" ht="50.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="20" t="s">
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+    </row>
+    <row r="21" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="21" t="s">
         <v>250</v>
       </c>
-      <c r="B19" s="20"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-    </row>
-    <row r="20" spans="1:4" ht="77.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="20" t="s">
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+    </row>
+    <row r="22" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A22" s="21" t="s">
         <v>251</v>
       </c>
-      <c r="B20" s="20"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
-    </row>
-    <row r="21" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="20" t="s">
+      <c r="B22" s="21"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+    </row>
+    <row r="23" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A23" s="87" t="s">
         <v>252</v>
       </c>
-      <c r="B21" s="20"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-    </row>
-    <row r="22" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="20" t="s">
-        <v>253</v>
-      </c>
-      <c r="B22" s="20"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-    </row>
-    <row r="23" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="83" t="s">
-        <v>254</v>
-      </c>
-      <c r="B23" s="83"/>
-      <c r="C23" s="83"/>
-      <c r="D23" s="83"/>
+      <c r="B23" s="87"/>
+      <c r="C23" s="87"/>
+      <c r="D23" s="87"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -6942,354 +6943,354 @@
       <selection sqref="A1:H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="39.5" customWidth="1"/>
+    <col min="1" max="1" width="39.46875" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="45.33203125" customWidth="1"/>
-    <col min="4" max="4" width="6.83203125" customWidth="1"/>
-    <col min="5" max="5" width="7.1640625" customWidth="1"/>
-    <col min="6" max="7" width="1.33203125" customWidth="1"/>
-    <col min="8" max="8" width="6.83203125" customWidth="1"/>
+    <col min="3" max="3" width="45.3515625" customWidth="1"/>
+    <col min="4" max="4" width="6.8203125" customWidth="1"/>
+    <col min="5" max="5" width="7.17578125" customWidth="1"/>
+    <col min="6" max="7" width="1.3515625" customWidth="1"/>
+    <col min="8" max="8" width="6.8203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:8" ht="37" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-    </row>
-    <row r="2" spans="1:8" ht="191.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="20" t="s">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+    </row>
+    <row r="2" spans="1:8" ht="191.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-    </row>
-    <row r="3" spans="1:8" ht="39.200000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="20" t="s">
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+    </row>
+    <row r="3" spans="1:8" ht="39.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-    </row>
-    <row r="4" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+    </row>
+    <row r="4" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="28" t="s">
+    <row r="5" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
       <c r="F5" s="7"/>
     </row>
-    <row r="6" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="28" t="s">
+    <row r="6" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="28" t="s">
+    <row r="7" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-    </row>
-    <row r="8" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="30" t="s">
+      <c r="B7" s="29"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+    </row>
+    <row r="8" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="30"/>
-      <c r="C8" s="31" t="s">
+      <c r="B8" s="31"/>
+      <c r="C8" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-    </row>
-    <row r="9" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="20" t="s">
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
+    </row>
+    <row r="9" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-    </row>
-    <row r="10" spans="1:8" ht="97.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="20" t="s">
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+    </row>
+    <row r="10" spans="1:8" ht="97.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-    </row>
-    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="27" t="s">
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
+    </row>
+    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="27"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
-    </row>
-    <row r="12" spans="1:8" ht="133.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="20" t="s">
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+    </row>
+    <row r="12" spans="1:8" ht="133.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-    </row>
-    <row r="13" spans="1:8" ht="339.95" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:8" ht="267" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="20" t="s">
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+    </row>
+    <row r="13" spans="1:8" ht="340" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="14" spans="1:8" ht="267" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A14" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="20"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-    </row>
-    <row r="15" spans="1:8" ht="219" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="27" t="s">
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+    </row>
+    <row r="15" spans="1:8" ht="219" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A16" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="27"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="27"/>
-    </row>
-    <row r="17" spans="1:8" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="20" t="s">
+      <c r="B16" s="28"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="28"/>
+    </row>
+    <row r="17" spans="1:8" ht="68.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A17" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="20"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
-    </row>
-    <row r="18" spans="1:8" ht="91.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="20" t="s">
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="21"/>
+    </row>
+    <row r="18" spans="1:8" ht="91.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A18" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="20"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
-    </row>
-    <row r="19" spans="1:8" ht="77.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="20" t="s">
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
+    </row>
+    <row r="19" spans="1:8" ht="77.099999999999994" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A19" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="20"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-    </row>
-    <row r="20" spans="1:8" ht="91.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="20" t="s">
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+    </row>
+    <row r="20" spans="1:8" ht="91.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="20"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
-    </row>
-    <row r="21" spans="1:8" ht="198" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" spans="1:8" ht="77.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="20" t="s">
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
+    </row>
+    <row r="21" spans="1:8" ht="198" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="22" spans="1:8" ht="77.099999999999994" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A22" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="20"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
-    </row>
-    <row r="23" spans="1:8" ht="77.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="20" t="s">
+      <c r="B22" s="21"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
+    </row>
+    <row r="23" spans="1:8" ht="77.099999999999994" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A23" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="B23" s="20"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
-    </row>
-    <row r="24" spans="1:8" ht="77.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="20" t="s">
+      <c r="B23" s="21"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="21"/>
+    </row>
+    <row r="24" spans="1:8" ht="77.099999999999994" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A24" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="20"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
-    </row>
-    <row r="25" spans="1:8" ht="47.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="20" t="s">
+      <c r="B24" s="21"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
+    </row>
+    <row r="25" spans="1:8" ht="47.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A25" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="B25" s="20"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="20"/>
-    </row>
-    <row r="26" spans="1:8" ht="77.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="20" t="s">
+      <c r="B25" s="21"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
+    </row>
+    <row r="26" spans="1:8" ht="77.099999999999994" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A26" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="B26" s="20"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20"/>
-    </row>
-    <row r="27" spans="1:8" ht="77.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="20" t="s">
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
+    </row>
+    <row r="27" spans="1:8" ht="77.099999999999994" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A27" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="B27" s="20"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20"/>
-    </row>
-    <row r="28" spans="1:8" ht="62.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="20" t="s">
+      <c r="B27" s="21"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+    </row>
+    <row r="28" spans="1:8" ht="62.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A28" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="B28" s="20"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="20"/>
-      <c r="G28" s="20"/>
-      <c r="H28" s="20"/>
-    </row>
-    <row r="29" spans="1:8" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="26" t="s">
+      <c r="B28" s="21"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="21"/>
+    </row>
+    <row r="29" spans="1:8" ht="37" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A29" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-    </row>
-    <row r="30" spans="1:8" ht="219" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="20" t="s">
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+    </row>
+    <row r="30" spans="1:8" ht="219" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A30" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-    </row>
-    <row r="31" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="27" t="s">
+      <c r="B30" s="21"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="21"/>
+      <c r="H30" s="21"/>
+    </row>
+    <row r="31" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A31" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="B31" s="27"/>
-      <c r="C31" s="27"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="27"/>
-      <c r="F31" s="27"/>
-      <c r="G31" s="27"/>
-      <c r="H31" s="27"/>
-    </row>
-    <row r="32" spans="1:8" ht="234.95" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="33" spans="1:7" ht="90.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="25" t="s">
+      <c r="B31" s="28"/>
+      <c r="C31" s="28"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="28"/>
+      <c r="H31" s="28"/>
+    </row>
+    <row r="32" spans="1:8" ht="235" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="33" spans="1:7" ht="90.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A33" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="B33" s="25"/>
-      <c r="C33" s="25"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="25"/>
-      <c r="F33" s="25"/>
-      <c r="G33" s="25"/>
+      <c r="B33" s="26"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="26"/>
+      <c r="F33" s="26"/>
+      <c r="G33" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="31">
@@ -7343,84 +7344,84 @@
       <selection sqref="A1:H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.1640625" customWidth="1"/>
-    <col min="2" max="2" width="56.83203125" customWidth="1"/>
-    <col min="3" max="3" width="28.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.1640625" customWidth="1"/>
+    <col min="1" max="1" width="16.17578125" customWidth="1"/>
+    <col min="2" max="2" width="56.8203125" customWidth="1"/>
+    <col min="3" max="3" width="28.64453125" customWidth="1"/>
+    <col min="4" max="4" width="11.17578125" customWidth="1"/>
     <col min="5" max="5" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="36" t="s">
+    <row r="1" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-    </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="27" t="s">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+    </row>
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-    </row>
-    <row r="3" spans="1:5" ht="41.85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+    </row>
+    <row r="3" spans="1:5" ht="41.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="39"/>
-    </row>
-    <row r="4" spans="1:5" ht="23.85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C3" s="39"/>
+      <c r="D3" s="40"/>
+    </row>
+    <row r="4" spans="1:5" ht="23.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="34"/>
-      <c r="D4" s="35"/>
-    </row>
-    <row r="5" spans="1:5" ht="23.85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C4" s="35"/>
+      <c r="D4" s="36"/>
+    </row>
+    <row r="5" spans="1:5" ht="23.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="34"/>
-      <c r="D5" s="35"/>
-    </row>
-    <row r="6" spans="1:5" ht="23.85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C5" s="35"/>
+      <c r="D5" s="36"/>
+    </row>
+    <row r="6" spans="1:5" ht="23.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="33" t="s">
+      <c r="B6" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="C6" s="34"/>
-      <c r="D6" s="35"/>
-    </row>
-    <row r="7" spans="1:5" ht="23.85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C6" s="35"/>
+      <c r="D6" s="36"/>
+    </row>
+    <row r="7" spans="1:5" ht="23.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="C7" s="34"/>
-      <c r="D7" s="35"/>
-    </row>
-    <row r="8" spans="1:5" ht="23.85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C7" s="35"/>
+      <c r="D7" s="36"/>
+    </row>
+    <row r="8" spans="1:5" ht="23.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="11" t="s">
         <v>58</v>
       </c>
@@ -7434,7 +7435,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="23.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="23.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="8" t="s">
         <v>62</v>
       </c>
@@ -7446,7 +7447,7 @@
       </c>
       <c r="D9" s="12"/>
     </row>
-    <row r="10" spans="1:5" ht="77.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="77.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="9" t="s">
         <v>65</v>
       </c>
@@ -7460,7 +7461,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="71.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="71.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="9" t="s">
         <v>69</v>
       </c>
@@ -7496,97 +7497,97 @@
       <selection sqref="A1:H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.5" customWidth="1"/>
-    <col min="2" max="2" width="21.5" customWidth="1"/>
-    <col min="3" max="3" width="29.83203125" customWidth="1"/>
-    <col min="4" max="4" width="17.5" customWidth="1"/>
+    <col min="1" max="1" width="16.46875" customWidth="1"/>
+    <col min="2" max="2" width="21.46875" customWidth="1"/>
+    <col min="3" max="3" width="29.8203125" customWidth="1"/>
+    <col min="4" max="4" width="17.46875" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="11.1640625" customWidth="1"/>
+    <col min="6" max="6" width="11.17578125" customWidth="1"/>
     <col min="7" max="7" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="153.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:7" ht="153.6" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-    </row>
-    <row r="2" spans="1:7" ht="41.85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+    </row>
+    <row r="2" spans="1:7" ht="41.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="39"/>
-    </row>
-    <row r="3" spans="1:7" ht="23.85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="40"/>
+    </row>
+    <row r="3" spans="1:7" ht="23.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="35"/>
-    </row>
-    <row r="4" spans="1:7" ht="23.85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="36"/>
+    </row>
+    <row r="4" spans="1:7" ht="23.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="35"/>
-    </row>
-    <row r="5" spans="1:7" ht="23.85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="36"/>
+    </row>
+    <row r="5" spans="1:7" ht="23.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="35"/>
-    </row>
-    <row r="6" spans="1:7" ht="35.85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="36"/>
+    </row>
+    <row r="6" spans="1:7" ht="35.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="B6" s="33" t="s">
+      <c r="B6" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="35"/>
-    </row>
-    <row r="7" spans="1:7" ht="23.85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="36"/>
+    </row>
+    <row r="7" spans="1:7" ht="23.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="B7" s="45" t="s">
+      <c r="B7" s="46" t="s">
         <v>59</v>
       </c>
-      <c r="C7" s="46"/>
-      <c r="D7" s="47"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="48"/>
       <c r="E7" s="11" t="s">
         <v>60</v>
       </c>
@@ -7594,153 +7595,153 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="23.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="23.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="B8" s="48" t="s">
+      <c r="B8" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="C8" s="49"/>
-      <c r="D8" s="50"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="51"/>
       <c r="E8" s="8" t="s">
         <v>77</v>
       </c>
       <c r="F8" s="12"/>
     </row>
-    <row r="9" spans="1:7" ht="68.849999999999994" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="68.849999999999994" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="B9" s="51" t="s">
+      <c r="B9" s="52" t="s">
         <v>79</v>
       </c>
-      <c r="C9" s="52"/>
-      <c r="D9" s="53"/>
-      <c r="E9" s="54" t="s">
+      <c r="C9" s="53"/>
+      <c r="D9" s="54"/>
+      <c r="E9" s="55" t="s">
         <v>80</v>
       </c>
-      <c r="F9" s="57" t="s">
+      <c r="F9" s="58" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="18.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="40"/>
+    <row r="10" spans="1:7" ht="18.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="41"/>
       <c r="B10" s="15" t="s">
         <v>82</v>
       </c>
       <c r="C10" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="D10" s="41"/>
-      <c r="E10" s="55"/>
-      <c r="F10" s="58"/>
-    </row>
-    <row r="11" spans="1:7" ht="18.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="40"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="59"/>
+    </row>
+    <row r="11" spans="1:7" ht="18.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="41"/>
       <c r="B11" s="16" t="s">
         <v>84</v>
       </c>
       <c r="C11" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="D11" s="41"/>
-      <c r="E11" s="55"/>
-      <c r="F11" s="58"/>
-    </row>
-    <row r="12" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="40"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="56"/>
+      <c r="F11" s="59"/>
+    </row>
+    <row r="12" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="41"/>
       <c r="B12" s="16" t="s">
         <v>86</v>
       </c>
       <c r="C12" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="D12" s="41"/>
-      <c r="E12" s="55"/>
-      <c r="F12" s="58"/>
-    </row>
-    <row r="13" spans="1:7" ht="18.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="40"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="59"/>
+    </row>
+    <row r="13" spans="1:7" ht="18.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="41"/>
       <c r="B13" s="16" t="s">
         <v>88</v>
       </c>
       <c r="C13" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="D13" s="41"/>
-      <c r="E13" s="55"/>
-      <c r="F13" s="58"/>
-    </row>
-    <row r="14" spans="1:7" ht="18.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="40"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="56"/>
+      <c r="F13" s="59"/>
+    </row>
+    <row r="14" spans="1:7" ht="18.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A14" s="41"/>
       <c r="B14" s="16" t="s">
         <v>90</v>
       </c>
       <c r="C14" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="D14" s="41"/>
-      <c r="E14" s="55"/>
-      <c r="F14" s="58"/>
-    </row>
-    <row r="15" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="40"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="56"/>
+      <c r="F14" s="59"/>
+    </row>
+    <row r="15" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="41"/>
       <c r="B15" s="16" t="s">
         <v>92</v>
       </c>
       <c r="C15" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="D15" s="41"/>
-      <c r="E15" s="55"/>
-      <c r="F15" s="58"/>
-    </row>
-    <row r="16" spans="1:7" ht="18.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="40"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="59"/>
+    </row>
+    <row r="16" spans="1:7" ht="18.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A16" s="41"/>
       <c r="B16" s="16" t="s">
         <v>94</v>
       </c>
       <c r="C16" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="D16" s="41"/>
-      <c r="E16" s="55"/>
-      <c r="F16" s="58"/>
-    </row>
-    <row r="17" spans="1:6" ht="18.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="40"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="59"/>
+    </row>
+    <row r="17" spans="1:6" ht="18.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A17" s="41"/>
       <c r="B17" s="16" t="s">
         <v>96</v>
       </c>
       <c r="C17" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="D17" s="41"/>
-      <c r="E17" s="55"/>
-      <c r="F17" s="58"/>
-    </row>
-    <row r="18" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="40"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="56"/>
+      <c r="F17" s="59"/>
+    </row>
+    <row r="18" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A18" s="41"/>
       <c r="B18" s="16" t="s">
         <v>98</v>
       </c>
       <c r="C18" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="D18" s="41"/>
-      <c r="E18" s="55"/>
-      <c r="F18" s="58"/>
-    </row>
-    <row r="19" spans="1:6" ht="86.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D18" s="42"/>
+      <c r="E18" s="56"/>
+      <c r="F18" s="59"/>
+    </row>
+    <row r="19" spans="1:6" ht="86.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="14"/>
-      <c r="B19" s="42" t="s">
+      <c r="B19" s="43" t="s">
         <v>100</v>
       </c>
-      <c r="C19" s="43"/>
-      <c r="D19" s="44"/>
-      <c r="E19" s="56"/>
-      <c r="F19" s="59"/>
+      <c r="C19" s="44"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="57"/>
+      <c r="F19" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -7767,45 +7768,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H19"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.5" customWidth="1"/>
-    <col min="2" max="2" width="21.5" customWidth="1"/>
-    <col min="3" max="3" width="16.1640625" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" customWidth="1"/>
+    <col min="1" max="1" width="16.46875" customWidth="1"/>
+    <col min="2" max="2" width="21.46875" customWidth="1"/>
+    <col min="3" max="3" width="16.17578125" customWidth="1"/>
+    <col min="4" max="4" width="13.3515625" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="1.5" customWidth="1"/>
+    <col min="6" max="6" width="1.46875" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
-    <col min="8" max="8" width="11.1640625" customWidth="1"/>
+    <col min="8" max="8" width="11.17578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="35.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="35.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="17"/>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="36"/>
       <c r="G1" s="17"/>
       <c r="H1" s="17"/>
     </row>
-    <row r="2" spans="1:8" ht="59.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="59.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="38" t="s">
         <v>103</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="40"/>
       <c r="G2" s="10" t="s">
         <v>104</v>
       </c>
@@ -7813,173 +7812,173 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="68.849999999999994" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="68.849999999999994" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="52" t="s">
         <v>106</v>
       </c>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="57" t="s">
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="58" t="s">
         <v>107</v>
       </c>
-      <c r="H3" s="71">
+      <c r="H3" s="72">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="18.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="40"/>
+    <row r="4" spans="1:8" ht="18.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="41"/>
       <c r="B4" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="C4" s="66" t="s">
+      <c r="C4" s="67" t="s">
         <v>83</v>
       </c>
-      <c r="D4" s="67"/>
-      <c r="E4" s="69"/>
-      <c r="F4" s="70"/>
-      <c r="G4" s="58"/>
-      <c r="H4" s="72"/>
-    </row>
-    <row r="5" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="40"/>
+      <c r="D4" s="68"/>
+      <c r="E4" s="70"/>
+      <c r="F4" s="71"/>
+      <c r="G4" s="59"/>
+      <c r="H4" s="73"/>
+    </row>
+    <row r="5" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="41"/>
       <c r="B5" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="C5" s="60" t="s">
+      <c r="C5" s="61" t="s">
         <v>109</v>
       </c>
-      <c r="D5" s="61"/>
-      <c r="E5" s="69"/>
-      <c r="F5" s="70"/>
-      <c r="G5" s="58"/>
-      <c r="H5" s="72"/>
-    </row>
-    <row r="6" spans="1:8" ht="18.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="40"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="70"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="59"/>
+      <c r="H5" s="73"/>
+    </row>
+    <row r="6" spans="1:8" ht="18.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="41"/>
       <c r="B6" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="C6" s="60" t="s">
+      <c r="C6" s="61" t="s">
         <v>111</v>
       </c>
-      <c r="D6" s="61"/>
-      <c r="E6" s="69"/>
-      <c r="F6" s="70"/>
-      <c r="G6" s="58"/>
-      <c r="H6" s="72"/>
-    </row>
-    <row r="7" spans="1:8" ht="18.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="40"/>
+      <c r="D6" s="62"/>
+      <c r="E6" s="70"/>
+      <c r="F6" s="71"/>
+      <c r="G6" s="59"/>
+      <c r="H6" s="73"/>
+    </row>
+    <row r="7" spans="1:8" ht="18.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="41"/>
       <c r="B7" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="C7" s="60" t="s">
+      <c r="C7" s="61" t="s">
         <v>113</v>
       </c>
-      <c r="D7" s="61"/>
-      <c r="E7" s="69"/>
-      <c r="F7" s="70"/>
-      <c r="G7" s="58"/>
-      <c r="H7" s="72"/>
-    </row>
-    <row r="8" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="40"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="70"/>
+      <c r="F7" s="71"/>
+      <c r="G7" s="59"/>
+      <c r="H7" s="73"/>
+    </row>
+    <row r="8" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="41"/>
       <c r="B8" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="C8" s="60" t="s">
+      <c r="C8" s="61" t="s">
         <v>115</v>
       </c>
-      <c r="D8" s="61"/>
-      <c r="E8" s="69"/>
-      <c r="F8" s="70"/>
-      <c r="G8" s="58"/>
-      <c r="H8" s="72"/>
-    </row>
-    <row r="9" spans="1:8" ht="18.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="40"/>
+      <c r="D8" s="62"/>
+      <c r="E8" s="70"/>
+      <c r="F8" s="71"/>
+      <c r="G8" s="59"/>
+      <c r="H8" s="73"/>
+    </row>
+    <row r="9" spans="1:8" ht="18.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="41"/>
       <c r="B9" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="C9" s="60" t="s">
+      <c r="C9" s="61" t="s">
         <v>117</v>
       </c>
-      <c r="D9" s="61"/>
-      <c r="E9" s="69"/>
-      <c r="F9" s="70"/>
-      <c r="G9" s="58"/>
-      <c r="H9" s="72"/>
-    </row>
-    <row r="10" spans="1:8" ht="18.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="40"/>
+      <c r="D9" s="62"/>
+      <c r="E9" s="70"/>
+      <c r="F9" s="71"/>
+      <c r="G9" s="59"/>
+      <c r="H9" s="73"/>
+    </row>
+    <row r="10" spans="1:8" ht="18.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="41"/>
       <c r="B10" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="C10" s="60" t="s">
+      <c r="C10" s="61" t="s">
         <v>119</v>
       </c>
-      <c r="D10" s="61"/>
-      <c r="E10" s="69"/>
-      <c r="F10" s="70"/>
-      <c r="G10" s="58"/>
-      <c r="H10" s="72"/>
-    </row>
-    <row r="11" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="40"/>
+      <c r="D10" s="62"/>
+      <c r="E10" s="70"/>
+      <c r="F10" s="71"/>
+      <c r="G10" s="59"/>
+      <c r="H10" s="73"/>
+    </row>
+    <row r="11" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="41"/>
       <c r="B11" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="C11" s="60" t="s">
+      <c r="C11" s="61" t="s">
         <v>121</v>
       </c>
-      <c r="D11" s="61"/>
-      <c r="E11" s="69"/>
-      <c r="F11" s="70"/>
-      <c r="G11" s="58"/>
-      <c r="H11" s="72"/>
-    </row>
-    <row r="12" spans="1:8" ht="18.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="40"/>
+      <c r="D11" s="62"/>
+      <c r="E11" s="70"/>
+      <c r="F11" s="71"/>
+      <c r="G11" s="59"/>
+      <c r="H11" s="73"/>
+    </row>
+    <row r="12" spans="1:8" ht="18.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="41"/>
       <c r="B12" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="C12" s="60" t="s">
+      <c r="C12" s="61" t="s">
         <v>123</v>
       </c>
-      <c r="D12" s="61"/>
-      <c r="E12" s="69"/>
-      <c r="F12" s="70"/>
-      <c r="G12" s="58"/>
-      <c r="H12" s="72"/>
-    </row>
-    <row r="13" spans="1:8" ht="50.85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D12" s="62"/>
+      <c r="E12" s="70"/>
+      <c r="F12" s="71"/>
+      <c r="G12" s="59"/>
+      <c r="H12" s="73"/>
+    </row>
+    <row r="13" spans="1:8" ht="50.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="14"/>
-      <c r="B13" s="42" t="s">
+      <c r="B13" s="43" t="s">
         <v>124</v>
       </c>
-      <c r="C13" s="43"/>
-      <c r="D13" s="43"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="44"/>
-      <c r="G13" s="59"/>
-      <c r="H13" s="73"/>
-    </row>
-    <row r="14" spans="1:8" ht="65.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C13" s="44"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="45"/>
+      <c r="G13" s="60"/>
+      <c r="H13" s="74"/>
+    </row>
+    <row r="14" spans="1:8" ht="65.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="B14" s="37" t="s">
+      <c r="B14" s="38" t="s">
         <v>126</v>
       </c>
-      <c r="C14" s="38"/>
-      <c r="D14" s="38"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="39"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="40"/>
       <c r="G14" s="10" t="s">
         <v>127</v>
       </c>
@@ -7987,135 +7986,135 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="80.849999999999994" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" ht="80.849999999999994" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="B15" s="62" t="s">
+      <c r="B15" s="63" t="s">
         <v>129</v>
       </c>
-      <c r="C15" s="63"/>
-      <c r="D15" s="63"/>
-      <c r="E15" s="63"/>
-      <c r="F15" s="64"/>
-      <c r="G15" s="54" t="s">
+      <c r="C15" s="64"/>
+      <c r="D15" s="64"/>
+      <c r="E15" s="64"/>
+      <c r="F15" s="65"/>
+      <c r="G15" s="55" t="s">
         <v>130</v>
       </c>
-      <c r="H15" s="57" t="s">
+      <c r="H15" s="58" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="18.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="40"/>
-      <c r="B16" s="66" t="s">
+    <row r="16" spans="1:8" ht="18.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A16" s="41"/>
+      <c r="B16" s="67" t="s">
         <v>82</v>
       </c>
-      <c r="C16" s="67"/>
-      <c r="D16" s="66" t="s">
+      <c r="C16" s="68"/>
+      <c r="D16" s="67" t="s">
         <v>83</v>
       </c>
-      <c r="E16" s="67"/>
-      <c r="F16" s="41"/>
-      <c r="G16" s="55"/>
-      <c r="H16" s="58"/>
-    </row>
-    <row r="17" spans="1:8" ht="30.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="40"/>
-      <c r="B17" s="60" t="s">
+      <c r="E16" s="68"/>
+      <c r="F16" s="42"/>
+      <c r="G16" s="56"/>
+      <c r="H16" s="59"/>
+    </row>
+    <row r="17" spans="1:8" ht="30.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A17" s="41"/>
+      <c r="B17" s="61" t="s">
         <v>131</v>
       </c>
-      <c r="C17" s="61"/>
-      <c r="D17" s="60" t="s">
+      <c r="C17" s="62"/>
+      <c r="D17" s="61" t="s">
         <v>132</v>
       </c>
-      <c r="E17" s="61"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="55"/>
-      <c r="H17" s="58"/>
-    </row>
-    <row r="18" spans="1:8" ht="30.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="40"/>
-      <c r="B18" s="60" t="s">
+      <c r="E17" s="62"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="56"/>
+      <c r="H17" s="59"/>
+    </row>
+    <row r="18" spans="1:8" ht="30.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A18" s="41"/>
+      <c r="B18" s="61" t="s">
         <v>133</v>
       </c>
-      <c r="C18" s="61"/>
-      <c r="D18" s="60" t="s">
+      <c r="C18" s="62"/>
+      <c r="D18" s="61" t="s">
         <v>134</v>
       </c>
-      <c r="E18" s="61"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="55"/>
-      <c r="H18" s="58"/>
-    </row>
-    <row r="19" spans="1:8" ht="18.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="40"/>
-      <c r="B19" s="60" t="s">
+      <c r="E18" s="62"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="56"/>
+      <c r="H18" s="59"/>
+    </row>
+    <row r="19" spans="1:8" ht="18.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A19" s="41"/>
+      <c r="B19" s="61" t="s">
         <v>135</v>
       </c>
-      <c r="C19" s="61"/>
-      <c r="D19" s="60" t="s">
+      <c r="C19" s="62"/>
+      <c r="D19" s="61" t="s">
         <v>136</v>
       </c>
-      <c r="E19" s="61"/>
-      <c r="F19" s="41"/>
-      <c r="G19" s="55"/>
-      <c r="H19" s="58"/>
-    </row>
-    <row r="20" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="40"/>
-      <c r="B20" s="60" t="s">
+      <c r="E19" s="62"/>
+      <c r="F19" s="42"/>
+      <c r="G19" s="56"/>
+      <c r="H19" s="59"/>
+    </row>
+    <row r="20" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="41"/>
+      <c r="B20" s="61" t="s">
         <v>137</v>
       </c>
-      <c r="C20" s="61"/>
-      <c r="D20" s="60" t="s">
+      <c r="C20" s="62"/>
+      <c r="D20" s="61" t="s">
         <v>138</v>
       </c>
-      <c r="E20" s="61"/>
-      <c r="F20" s="41"/>
-      <c r="G20" s="55"/>
-      <c r="H20" s="58"/>
-    </row>
-    <row r="21" spans="1:8" ht="18.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="40"/>
-      <c r="B21" s="60" t="s">
+      <c r="E20" s="62"/>
+      <c r="F20" s="42"/>
+      <c r="G20" s="56"/>
+      <c r="H20" s="59"/>
+    </row>
+    <row r="21" spans="1:8" ht="18.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="41"/>
+      <c r="B21" s="61" t="s">
         <v>139</v>
       </c>
-      <c r="C21" s="61"/>
-      <c r="D21" s="60" t="s">
+      <c r="C21" s="62"/>
+      <c r="D21" s="61" t="s">
         <v>140</v>
       </c>
-      <c r="E21" s="61"/>
-      <c r="F21" s="41"/>
-      <c r="G21" s="55"/>
-      <c r="H21" s="58"/>
-    </row>
-    <row r="22" spans="1:8" ht="18.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="40"/>
-      <c r="B22" s="60" t="s">
+      <c r="E21" s="62"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="56"/>
+      <c r="H21" s="59"/>
+    </row>
+    <row r="22" spans="1:8" ht="18.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A22" s="41"/>
+      <c r="B22" s="61" t="s">
         <v>141</v>
       </c>
-      <c r="C22" s="61"/>
-      <c r="D22" s="60" t="s">
+      <c r="C22" s="62"/>
+      <c r="D22" s="61" t="s">
         <v>142</v>
       </c>
-      <c r="E22" s="61"/>
-      <c r="F22" s="41"/>
-      <c r="G22" s="55"/>
-      <c r="H22" s="58"/>
-    </row>
-    <row r="23" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="65"/>
-      <c r="B23" s="60" t="s">
+      <c r="E22" s="62"/>
+      <c r="F22" s="42"/>
+      <c r="G22" s="56"/>
+      <c r="H22" s="59"/>
+    </row>
+    <row r="23" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A23" s="66"/>
+      <c r="B23" s="61" t="s">
         <v>143</v>
       </c>
-      <c r="C23" s="61"/>
-      <c r="D23" s="60" t="s">
+      <c r="C23" s="62"/>
+      <c r="D23" s="61" t="s">
         <v>144</v>
       </c>
-      <c r="E23" s="61"/>
-      <c r="F23" s="68"/>
-      <c r="G23" s="56"/>
-      <c r="H23" s="59"/>
+      <c r="E23" s="62"/>
+      <c r="F23" s="69"/>
+      <c r="G23" s="57"/>
+      <c r="H23" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="39">
@@ -8168,146 +8167,146 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H19"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.5" customWidth="1"/>
+    <col min="1" max="1" width="16.46875" customWidth="1"/>
     <col min="2" max="2" width="38" customWidth="1"/>
-    <col min="3" max="3" width="29.5" customWidth="1"/>
-    <col min="4" max="4" width="1.5" customWidth="1"/>
+    <col min="3" max="3" width="29.46875" customWidth="1"/>
+    <col min="4" max="4" width="1.46875" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="11.1640625" customWidth="1"/>
+    <col min="6" max="6" width="11.17578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="74"/>
+    <row r="1" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="75"/>
       <c r="B1" s="16" t="s">
         <v>145</v>
       </c>
       <c r="C1" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="D1" s="75"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-    </row>
-    <row r="2" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="40"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+    </row>
+    <row r="2" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="41"/>
       <c r="B2" s="16" t="s">
         <v>147</v>
       </c>
       <c r="C2" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="D2" s="41"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-    </row>
-    <row r="3" spans="1:6" ht="18.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="40"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+    </row>
+    <row r="3" spans="1:6" ht="18.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="41"/>
       <c r="B3" s="16" t="s">
         <v>149</v>
       </c>
       <c r="C3" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="D3" s="41"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-    </row>
-    <row r="4" spans="1:6" ht="18.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="40"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
+    </row>
+    <row r="4" spans="1:6" ht="18.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="41"/>
       <c r="B4" s="16" t="s">
         <v>151</v>
       </c>
       <c r="C4" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="D4" s="41"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
-    </row>
-    <row r="5" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="40"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="56"/>
+    </row>
+    <row r="5" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="41"/>
       <c r="B5" s="16" t="s">
         <v>153</v>
       </c>
       <c r="C5" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="D5" s="41"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="55"/>
-    </row>
-    <row r="6" spans="1:6" ht="18.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="40"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="56"/>
+      <c r="F5" s="56"/>
+    </row>
+    <row r="6" spans="1:6" ht="18.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="41"/>
       <c r="B6" s="16" t="s">
         <v>155</v>
       </c>
       <c r="C6" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="D6" s="41"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="55"/>
-    </row>
-    <row r="7" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="40"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="56"/>
+    </row>
+    <row r="7" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="41"/>
       <c r="B7" s="16" t="s">
         <v>157</v>
       </c>
       <c r="C7" s="16" t="s">
         <v>158</v>
       </c>
-      <c r="D7" s="41"/>
-      <c r="E7" s="55"/>
-      <c r="F7" s="55"/>
-    </row>
-    <row r="8" spans="1:6" ht="18.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="40"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="56"/>
+      <c r="F7" s="56"/>
+    </row>
+    <row r="8" spans="1:6" ht="18.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="41"/>
       <c r="B8" s="16" t="s">
         <v>159</v>
       </c>
       <c r="C8" s="16" t="s">
         <v>160</v>
       </c>
-      <c r="D8" s="41"/>
-      <c r="E8" s="55"/>
-      <c r="F8" s="55"/>
-    </row>
-    <row r="9" spans="1:6" ht="18.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="40"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="56"/>
+      <c r="F8" s="56"/>
+    </row>
+    <row r="9" spans="1:6" ht="18.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="41"/>
       <c r="B9" s="16" t="s">
         <v>161</v>
       </c>
       <c r="C9" s="16" t="s">
         <v>162</v>
       </c>
-      <c r="D9" s="41"/>
-      <c r="E9" s="55"/>
-      <c r="F9" s="55"/>
-    </row>
-    <row r="10" spans="1:6" ht="116.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D9" s="42"/>
+      <c r="E9" s="56"/>
+      <c r="F9" s="56"/>
+    </row>
+    <row r="10" spans="1:6" ht="116.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="14"/>
-      <c r="B10" s="76" t="s">
+      <c r="B10" s="77" t="s">
         <v>163</v>
       </c>
-      <c r="C10" s="77"/>
-      <c r="D10" s="78"/>
-      <c r="E10" s="56"/>
-      <c r="F10" s="56"/>
-    </row>
-    <row r="11" spans="1:6" ht="119.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C10" s="78"/>
+      <c r="D10" s="79"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="57"/>
+    </row>
+    <row r="11" spans="1:6" ht="119.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="10" t="s">
         <v>164</v>
       </c>
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="38" t="s">
         <v>165</v>
       </c>
-      <c r="C11" s="38"/>
-      <c r="D11" s="39"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="40"/>
       <c r="E11" s="10" t="s">
         <v>166</v>
       </c>
@@ -8315,15 +8314,15 @@
         <v>167</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="59.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="9" t="s">
+    <row r="12" spans="1:6" ht="59.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="20" t="s">
+        <v>254</v>
+      </c>
+      <c r="B12" s="38" t="s">
         <v>168</v>
       </c>
-      <c r="B12" s="37" t="s">
-        <v>169</v>
-      </c>
-      <c r="C12" s="38"/>
-      <c r="D12" s="39"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="40"/>
       <c r="E12" s="10" t="s">
         <v>67</v>
       </c>
@@ -8331,33 +8330,33 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="41.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="41.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="B13" s="34" t="s">
         <v>170</v>
       </c>
-      <c r="B13" s="33" t="s">
+      <c r="C13" s="35"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="10" t="s">
         <v>171</v>
-      </c>
-      <c r="C13" s="34"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="10" t="s">
-        <v>172</v>
       </c>
       <c r="F13" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="53.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="53.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="B14" s="38" t="s">
         <v>173</v>
       </c>
-      <c r="B14" s="37" t="s">
-        <v>174</v>
-      </c>
-      <c r="C14" s="38"/>
-      <c r="D14" s="39"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="40"/>
       <c r="E14" s="10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F14" s="10" t="s">
         <v>167</v>
@@ -8365,7 +8364,6 @@
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="E1:E10"/>
     <mergeCell ref="F1:F10"/>
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="B11:D11"/>
@@ -8374,6 +8372,7 @@
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="A1:A9"/>
     <mergeCell ref="D1:D9"/>
+    <mergeCell ref="E1:E10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8383,101 +8382,101 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H22"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.5" customWidth="1"/>
-    <col min="2" max="2" width="28.1640625" customWidth="1"/>
-    <col min="3" max="3" width="26.5" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" customWidth="1"/>
-    <col min="5" max="5" width="17.5" customWidth="1"/>
-    <col min="6" max="6" width="11.1640625" customWidth="1"/>
+    <col min="1" max="1" width="16.46875" customWidth="1"/>
+    <col min="2" max="2" width="28.17578125" customWidth="1"/>
+    <col min="3" max="3" width="26.46875" customWidth="1"/>
+    <col min="4" max="4" width="12.64453125" customWidth="1"/>
+    <col min="5" max="5" width="17.46875" customWidth="1"/>
+    <col min="6" max="6" width="11.17578125" customWidth="1"/>
     <col min="7" max="7" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="81.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
-        <v>175</v>
-      </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-    </row>
-    <row r="2" spans="1:7" ht="41.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="81.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+    </row>
+    <row r="2" spans="1:7" ht="41.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="37" t="s">
-        <v>176</v>
-      </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="39"/>
-    </row>
-    <row r="3" spans="1:7" ht="23.85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="38" t="s">
+        <v>175</v>
+      </c>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="40"/>
+    </row>
+    <row r="3" spans="1:7" ht="23.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="35"/>
-    </row>
-    <row r="4" spans="1:7" ht="23.85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="36"/>
+    </row>
+    <row r="4" spans="1:7" ht="23.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="B4" s="33" t="s">
-        <v>177</v>
-      </c>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="35"/>
-    </row>
-    <row r="5" spans="1:7" ht="23.85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="36"/>
+    </row>
+    <row r="5" spans="1:7" ht="23.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="35"/>
-    </row>
-    <row r="6" spans="1:7" ht="23.85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="36"/>
+    </row>
+    <row r="6" spans="1:7" ht="23.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="B6" s="33" t="s">
-        <v>178</v>
-      </c>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="35"/>
-    </row>
-    <row r="7" spans="1:7" ht="23.85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="34" t="s">
+        <v>177</v>
+      </c>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="36"/>
+    </row>
+    <row r="7" spans="1:7" ht="23.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="B7" s="45" t="s">
+      <c r="B7" s="46" t="s">
         <v>59</v>
       </c>
-      <c r="C7" s="46"/>
-      <c r="D7" s="47"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="48"/>
       <c r="E7" s="11" t="s">
         <v>60</v>
       </c>
@@ -8485,199 +8484,199 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="23.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="23.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="B8" s="48" t="s">
+      <c r="B8" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="C8" s="49"/>
-      <c r="D8" s="50"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="51"/>
       <c r="E8" s="8" t="s">
         <v>77</v>
       </c>
       <c r="F8" s="12"/>
     </row>
-    <row r="9" spans="1:7" ht="68.849999999999994" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="68.849999999999994" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="B9" s="52" t="s">
         <v>179</v>
       </c>
-      <c r="B9" s="51" t="s">
+      <c r="C9" s="53"/>
+      <c r="D9" s="54"/>
+      <c r="E9" s="55" t="s">
         <v>180</v>
       </c>
-      <c r="C9" s="52"/>
-      <c r="D9" s="53"/>
-      <c r="E9" s="54" t="s">
-        <v>181</v>
-      </c>
-      <c r="F9" s="71">
+      <c r="F9" s="72">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="40"/>
+    <row r="10" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="41"/>
       <c r="B10" s="15" t="s">
         <v>82</v>
       </c>
       <c r="C10" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="D10" s="41"/>
-      <c r="E10" s="55"/>
-      <c r="F10" s="72"/>
-    </row>
-    <row r="11" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="65"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="73"/>
+    </row>
+    <row r="11" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="66"/>
       <c r="B11" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="C11" s="16" t="s">
         <v>182</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="D11" s="69"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="74"/>
+    </row>
+    <row r="12" spans="1:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="D11" s="68"/>
-      <c r="E11" s="56"/>
-      <c r="F11" s="73"/>
-    </row>
-    <row r="12" spans="1:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="10" t="s">
+      <c r="B12" s="80" t="s">
         <v>184</v>
       </c>
-      <c r="B12" s="79" t="s">
+      <c r="C12" s="81"/>
+      <c r="D12" s="82"/>
+      <c r="E12" s="10" t="s">
         <v>185</v>
-      </c>
-      <c r="C12" s="80"/>
-      <c r="D12" s="81"/>
-      <c r="E12" s="10" t="s">
-        <v>186</v>
       </c>
       <c r="F12" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="56.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="56.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="B13" s="52" t="s">
         <v>187</v>
       </c>
-      <c r="B13" s="51" t="s">
-        <v>188</v>
-      </c>
-      <c r="C13" s="52"/>
-      <c r="D13" s="53"/>
-      <c r="E13" s="57" t="s">
+      <c r="C13" s="53"/>
+      <c r="D13" s="54"/>
+      <c r="E13" s="58" t="s">
         <v>107</v>
       </c>
-      <c r="F13" s="71">
+      <c r="F13" s="72">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="40"/>
+    <row r="14" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A14" s="41"/>
       <c r="B14" s="15" t="s">
         <v>82</v>
       </c>
       <c r="C14" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="D14" s="41"/>
-      <c r="E14" s="58"/>
-      <c r="F14" s="72"/>
-    </row>
-    <row r="15" spans="1:7" ht="18.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="40"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="59"/>
+      <c r="F14" s="73"/>
+    </row>
+    <row r="15" spans="1:7" ht="18.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="41"/>
       <c r="B15" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C15" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="D15" s="41"/>
-      <c r="E15" s="58"/>
-      <c r="F15" s="72"/>
-    </row>
-    <row r="16" spans="1:7" ht="18.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="40"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="59"/>
+      <c r="F15" s="73"/>
+    </row>
+    <row r="16" spans="1:7" ht="18.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A16" s="41"/>
       <c r="B16" s="16" t="s">
         <v>110</v>
       </c>
       <c r="C16" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="D16" s="41"/>
-      <c r="E16" s="58"/>
-      <c r="F16" s="72"/>
-    </row>
-    <row r="17" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="40"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="59"/>
+      <c r="F16" s="73"/>
+    </row>
+    <row r="17" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A17" s="41"/>
       <c r="B17" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C17" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="D17" s="41"/>
-      <c r="E17" s="58"/>
-      <c r="F17" s="72"/>
-    </row>
-    <row r="18" spans="1:6" ht="18.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="40"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="59"/>
+      <c r="F17" s="73"/>
+    </row>
+    <row r="18" spans="1:6" ht="18.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A18" s="41"/>
       <c r="B18" s="16" t="s">
         <v>114</v>
       </c>
       <c r="C18" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="D18" s="41"/>
-      <c r="E18" s="58"/>
-      <c r="F18" s="72"/>
-    </row>
-    <row r="19" spans="1:6" ht="18.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="40"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="59"/>
+      <c r="F18" s="73"/>
+    </row>
+    <row r="19" spans="1:6" ht="18.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A19" s="41"/>
       <c r="B19" s="16" t="s">
         <v>116</v>
       </c>
       <c r="C19" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="D19" s="41"/>
-      <c r="E19" s="58"/>
-      <c r="F19" s="72"/>
-    </row>
-    <row r="20" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="40"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="59"/>
+      <c r="F19" s="73"/>
+    </row>
+    <row r="20" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="41"/>
       <c r="B20" s="16" t="s">
         <v>118</v>
       </c>
       <c r="C20" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="D20" s="41"/>
-      <c r="E20" s="58"/>
-      <c r="F20" s="72"/>
-    </row>
-    <row r="21" spans="1:6" ht="18.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="40"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="59"/>
+      <c r="F20" s="73"/>
+    </row>
+    <row r="21" spans="1:6" ht="18.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="41"/>
       <c r="B21" s="16" t="s">
         <v>120</v>
       </c>
       <c r="C21" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="D21" s="41"/>
-      <c r="E21" s="58"/>
-      <c r="F21" s="72"/>
-    </row>
-    <row r="22" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="65"/>
+      <c r="D21" s="42"/>
+      <c r="E21" s="59"/>
+      <c r="F21" s="73"/>
+    </row>
+    <row r="22" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A22" s="66"/>
       <c r="B22" s="16" t="s">
         <v>122</v>
       </c>
       <c r="C22" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="D22" s="68"/>
-      <c r="E22" s="59"/>
-      <c r="F22" s="73"/>
+      <c r="D22" s="69"/>
+      <c r="E22" s="60"/>
+      <c r="F22" s="74"/>
     </row>
   </sheetData>
   <mergeCells count="19">
@@ -8709,109 +8708,109 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:D8"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.5" customWidth="1"/>
-    <col min="2" max="2" width="28.1640625" customWidth="1"/>
-    <col min="3" max="3" width="26.5" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" customWidth="1"/>
-    <col min="5" max="5" width="17.5" customWidth="1"/>
-    <col min="6" max="6" width="11.1640625" customWidth="1"/>
+    <col min="1" max="1" width="16.46875" customWidth="1"/>
+    <col min="2" max="2" width="28.17578125" customWidth="1"/>
+    <col min="3" max="3" width="26.46875" customWidth="1"/>
+    <col min="4" max="4" width="12.64453125" customWidth="1"/>
+    <col min="5" max="5" width="17.46875" customWidth="1"/>
+    <col min="6" max="6" width="11.17578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="65.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="65.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="B1" s="38" t="s">
         <v>189</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="C1" s="39"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="10" t="s">
         <v>190</v>
-      </c>
-      <c r="C1" s="38"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="10" t="s">
-        <v>191</v>
       </c>
       <c r="F1" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="80.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="80.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="B2" s="52" t="s">
         <v>192</v>
       </c>
-      <c r="B2" s="51" t="s">
+      <c r="C2" s="53"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="55" t="s">
         <v>193</v>
       </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="54" t="s">
+      <c r="F2" s="58" t="s">
         <v>194</v>
       </c>
-      <c r="F2" s="57" t="s">
+    </row>
+    <row r="3" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="41"/>
+      <c r="B3" s="15" t="s">
         <v>195</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="40"/>
-      <c r="B3" s="15" t="s">
-        <v>196</v>
       </c>
       <c r="C3" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="D3" s="41"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="58"/>
-    </row>
-    <row r="4" spans="1:6" ht="18.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="40"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="59"/>
+    </row>
+    <row r="4" spans="1:6" ht="18.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="41"/>
       <c r="B4" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="C4" s="16" t="s">
         <v>197</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="D4" s="42"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="59"/>
+    </row>
+    <row r="5" spans="1:6" ht="18.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="41"/>
+      <c r="B5" s="16" t="s">
         <v>198</v>
       </c>
-      <c r="D4" s="41"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="58"/>
-    </row>
-    <row r="5" spans="1:6" ht="18.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="40"/>
-      <c r="B5" s="16" t="s">
+      <c r="C5" s="16" t="s">
         <v>199</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="D5" s="42"/>
+      <c r="E5" s="56"/>
+      <c r="F5" s="59"/>
+    </row>
+    <row r="6" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="66"/>
+      <c r="B6" s="16" t="s">
         <v>200</v>
       </c>
-      <c r="D5" s="41"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="58"/>
-    </row>
-    <row r="6" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="65"/>
-      <c r="B6" s="16" t="s">
+      <c r="C6" s="16" t="s">
         <v>201</v>
       </c>
-      <c r="C6" s="16" t="s">
-        <v>202</v>
-      </c>
-      <c r="D6" s="68"/>
-      <c r="E6" s="56"/>
-      <c r="F6" s="59"/>
-    </row>
-    <row r="7" spans="1:6" ht="132.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D6" s="69"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="60"/>
+    </row>
+    <row r="7" spans="1:6" ht="132.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="10" t="s">
         <v>164</v>
       </c>
-      <c r="B7" s="82" t="s">
-        <v>255</v>
-      </c>
-      <c r="C7" s="80"/>
-      <c r="D7" s="81"/>
+      <c r="B7" s="83" t="s">
+        <v>253</v>
+      </c>
+      <c r="C7" s="81"/>
+      <c r="D7" s="82"/>
       <c r="E7" s="10" t="s">
         <v>166</v>
       </c>
@@ -8819,15 +8818,15 @@
         <v>167</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="65.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="65.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="B8" s="38" t="s">
         <v>203</v>
       </c>
-      <c r="B8" s="37" t="s">
-        <v>204</v>
-      </c>
-      <c r="C8" s="38"/>
-      <c r="D8" s="39"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="40"/>
       <c r="E8" s="10" t="s">
         <v>67</v>
       </c>
@@ -8835,15 +8834,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="65.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="65.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="B9" s="38" t="s">
         <v>205</v>
       </c>
-      <c r="B9" s="37" t="s">
-        <v>206</v>
-      </c>
-      <c r="C9" s="38"/>
-      <c r="D9" s="39"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="40"/>
       <c r="E9" s="10" t="s">
         <v>67</v>
       </c>
@@ -8851,33 +8850,33 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="41.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="41.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="B10" s="34" t="s">
         <v>170</v>
       </c>
-      <c r="B10" s="33" t="s">
+      <c r="C10" s="35"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="10" t="s">
         <v>171</v>
-      </c>
-      <c r="C10" s="34"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="10" t="s">
-        <v>172</v>
       </c>
       <c r="F10" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="53.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="53.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="B11" s="38" t="s">
         <v>173</v>
       </c>
-      <c r="B11" s="37" t="s">
-        <v>174</v>
-      </c>
-      <c r="C11" s="38"/>
-      <c r="D11" s="39"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="40"/>
       <c r="E11" s="10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F11" s="10" t="s">
         <v>167</v>
@@ -8905,79 +8904,79 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.1640625" customWidth="1"/>
-    <col min="2" max="2" width="66.1640625" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" customWidth="1"/>
-    <col min="4" max="4" width="11.1640625" customWidth="1"/>
+    <col min="1" max="1" width="16.17578125" customWidth="1"/>
+    <col min="2" max="2" width="66.17578125" customWidth="1"/>
+    <col min="3" max="3" width="19.3515625" customWidth="1"/>
+    <col min="4" max="4" width="11.17578125" customWidth="1"/>
     <col min="5" max="5" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="54.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
-        <v>207</v>
-      </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-    </row>
-    <row r="2" spans="1:5" ht="23.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="55" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="21" t="s">
+        <v>206</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+    </row>
+    <row r="2" spans="1:5" ht="23.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="33" t="s">
-        <v>208</v>
-      </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="35"/>
-    </row>
-    <row r="3" spans="1:5" ht="23.85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="84" t="s">
+        <v>255</v>
+      </c>
+      <c r="C2" s="85"/>
+      <c r="D2" s="86"/>
+    </row>
+    <row r="3" spans="1:5" ht="23.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="34"/>
-      <c r="D3" s="35"/>
-    </row>
-    <row r="4" spans="1:5" ht="23.85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C3" s="35"/>
+      <c r="D3" s="36"/>
+    </row>
+    <row r="4" spans="1:5" ht="23.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="B4" s="33" t="s">
-        <v>209</v>
-      </c>
-      <c r="C4" s="34"/>
-      <c r="D4" s="35"/>
-    </row>
-    <row r="5" spans="1:5" ht="23.85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="34" t="s">
+        <v>207</v>
+      </c>
+      <c r="C4" s="35"/>
+      <c r="D4" s="36"/>
+    </row>
+    <row r="5" spans="1:5" ht="23.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="B5" s="33" t="s">
-        <v>210</v>
-      </c>
-      <c r="C5" s="34"/>
-      <c r="D5" s="35"/>
-    </row>
-    <row r="6" spans="1:5" ht="23.85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="34" t="s">
+        <v>208</v>
+      </c>
+      <c r="C5" s="35"/>
+      <c r="D5" s="36"/>
+    </row>
+    <row r="6" spans="1:5" ht="23.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="B6" s="33" t="s">
-        <v>211</v>
-      </c>
-      <c r="C6" s="34"/>
-      <c r="D6" s="35"/>
-    </row>
-    <row r="7" spans="1:5" ht="23.85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="34" t="s">
+        <v>209</v>
+      </c>
+      <c r="C6" s="35"/>
+      <c r="D6" s="36"/>
+    </row>
+    <row r="7" spans="1:5" ht="23.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="11" t="s">
         <v>58</v>
       </c>
@@ -8991,7 +8990,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="23.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="23.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="8" t="s">
         <v>62</v>
       </c>
@@ -9003,71 +9002,71 @@
       </c>
       <c r="D8" s="12"/>
     </row>
-    <row r="9" spans="1:5" ht="41.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="41.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="C9" s="10" t="s">
         <v>212</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>213</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>214</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="53.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="53.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="C10" s="10" t="s">
         <v>215</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>216</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>217</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="41.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="41.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="C11" s="10" t="s">
         <v>218</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>219</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>220</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="41.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="41.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="C12" s="10" t="s">
         <v>221</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>222</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>223</v>
       </c>
       <c r="D12" s="10" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="41.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="41.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="C13" s="10" t="s">
         <v>224</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>226</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>167</v>

</xml_diff>